<commit_message>
Comment and disable special arrangements
</commit_message>
<xml_diff>
--- a/SampleData_RealAnon2020/forBot_FacultyAvailabilityMatrix.xlsx
+++ b/SampleData_RealAnon2020/forBot_FacultyAvailabilityMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/SampleData_RealAnon2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A2D89E9-4E54-4A7D-8F24-66A1354EA094}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD7AF21-B9DE-3843-8148-48BFD16857D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="67940" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="148">
   <si>
     <t>Scott Atwood</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>Tuesday, Feb. 11 3:15 - 3:45</t>
-  </si>
-  <si>
-    <t>Tuesday, Feb. 11 3:30 - 4:00</t>
   </si>
   <si>
     <t>Tuesday, Feb. 11 3:45 - 4:15</t>
@@ -1038,341 +1035,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW15"/>
+  <dimension ref="A1:AW14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L13" sqref="L13"/>
+      <selection pane="topRight" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.875" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="4" width="17.625" customWidth="1"/>
-    <col min="5" max="5" width="18.375" customWidth="1"/>
-    <col min="6" max="7" width="14.125" customWidth="1"/>
-    <col min="8" max="8" width="17.75" customWidth="1"/>
-    <col min="9" max="9" width="13.25" customWidth="1"/>
-    <col min="10" max="10" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="7" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
     <col min="11" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="14.875" customWidth="1"/>
-    <col min="15" max="15" width="14.125" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
     <col min="16" max="16" width="17.5" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="14.25" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" customWidth="1"/>
     <col min="19" max="20" width="15.5" customWidth="1"/>
-    <col min="21" max="21" width="12.875" customWidth="1"/>
-    <col min="22" max="22" width="15.75" customWidth="1"/>
-    <col min="23" max="23" width="15.25" style="21" customWidth="1"/>
-    <col min="24" max="25" width="16.25" customWidth="1"/>
+    <col min="21" max="21" width="12.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" style="21" customWidth="1"/>
+    <col min="24" max="25" width="16.1640625" customWidth="1"/>
     <col min="26" max="26" width="13.5" customWidth="1"/>
-    <col min="27" max="29" width="14.875" customWidth="1"/>
-    <col min="30" max="30" width="12.375" customWidth="1"/>
-    <col min="31" max="31" width="18.875" customWidth="1"/>
-    <col min="32" max="32" width="13.625" customWidth="1"/>
-    <col min="33" max="33" width="16.875" customWidth="1"/>
-    <col min="34" max="34" width="16.375" customWidth="1"/>
-    <col min="35" max="35" width="17.375" customWidth="1"/>
-    <col min="36" max="36" width="13.375" customWidth="1"/>
-    <col min="37" max="37" width="16.125" customWidth="1"/>
-    <col min="38" max="38" width="13.625" customWidth="1"/>
+    <col min="27" max="29" width="14.83203125" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+    <col min="31" max="31" width="18.83203125" customWidth="1"/>
+    <col min="32" max="32" width="13.6640625" customWidth="1"/>
+    <col min="33" max="33" width="16.83203125" customWidth="1"/>
+    <col min="34" max="34" width="16.33203125" customWidth="1"/>
+    <col min="35" max="35" width="17.33203125" customWidth="1"/>
+    <col min="36" max="36" width="13.33203125" customWidth="1"/>
+    <col min="37" max="37" width="16.1640625" customWidth="1"/>
+    <col min="38" max="38" width="13.6640625" customWidth="1"/>
     <col min="39" max="40" width="14" customWidth="1"/>
-    <col min="41" max="41" width="15.375" customWidth="1"/>
-    <col min="42" max="42" width="14.875" customWidth="1"/>
-    <col min="43" max="43" width="14.125" customWidth="1"/>
-    <col min="44" max="44" width="14.75" customWidth="1"/>
-    <col min="45" max="46" width="17.375" customWidth="1"/>
-    <col min="47" max="47" width="15.375" customWidth="1"/>
+    <col min="41" max="41" width="15.33203125" customWidth="1"/>
+    <col min="42" max="42" width="14.83203125" customWidth="1"/>
+    <col min="43" max="43" width="14.1640625" customWidth="1"/>
+    <col min="44" max="44" width="14.6640625" customWidth="1"/>
+    <col min="45" max="46" width="17.33203125" customWidth="1"/>
+    <col min="47" max="47" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S1" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T1" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U1" s="22" t="s">
         <v>9</v>
       </c>
       <c r="V1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="22" t="s">
-        <v>42</v>
-      </c>
       <c r="X1" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y1" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Z1" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA1" s="22" t="s">
         <v>11</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC1" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AD1" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE1" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF1" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" s="22" t="s">
+      <c r="AG1" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="AG1" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="22" t="s">
-        <v>86</v>
       </c>
       <c r="AI1" s="22" t="s">
         <v>14</v>
       </c>
       <c r="AJ1" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AK1" s="22" t="s">
         <v>15</v>
       </c>
       <c r="AL1" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="25" t="s">
-        <v>35</v>
-      </c>
       <c r="AN1" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AO1" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AP1" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AQ1" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AR1" s="22" t="s">
         <v>17</v>
       </c>
       <c r="AS1" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AT1" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AU1" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AV1" s="18"/>
       <c r="AW1" s="18"/>
     </row>
-    <row r="2" spans="1:49" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="F2" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y2" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA2" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC2" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE2" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF2" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ2" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK2" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="V2" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="W2" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="X2" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z2" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA2" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB2" s="26" t="s">
+      <c r="AL2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN2" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO2" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP2" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ2" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS2" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT2" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="AC2" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD2" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE2" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF2" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG2" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH2" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI2" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ2" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK2" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM2" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN2" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="AO2" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP2" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ2" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR2" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="AS2" s="25" t="s">
+      <c r="AU2" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="AT2" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="AU2" s="26" t="s">
-        <v>101</v>
       </c>
       <c r="AV2" s="18"/>
       <c r="AW2" s="18"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1455,7 +1452,7 @@
       <c r="AV3" s="18"/>
       <c r="AW3" s="18"/>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1544,7 +1541,7 @@
       <c r="AV4" s="18"/>
       <c r="AW4" s="18"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1641,7 +1638,7 @@
       <c r="AV5" s="18"/>
       <c r="AW5" s="18"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1732,7 +1729,7 @@
       <c r="AV6" s="18"/>
       <c r="AW6" s="18"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1813,7 +1810,7 @@
       <c r="AV7" s="18"/>
       <c r="AW7" s="18"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1888,7 +1885,7 @@
       <c r="AV8" s="18"/>
       <c r="AW8" s="18"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1987,7 +1984,7 @@
       <c r="AV9" s="18"/>
       <c r="AW9" s="18"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -2086,7 +2083,7 @@
       <c r="AV10" s="18"/>
       <c r="AW10" s="18"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -2191,7 +2188,7 @@
       <c r="AV11" s="18"/>
       <c r="AW11" s="18"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -2294,18 +2291,16 @@
       <c r="AV12" s="18"/>
       <c r="AW12" s="18"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2">
         <v>1</v>
       </c>
@@ -2313,9 +2308,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="17"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2">
-        <v>1</v>
-      </c>
+      <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="14"/>
       <c r="N13" s="3">
@@ -2327,22 +2320,20 @@
         <v>1</v>
       </c>
       <c r="R13" s="2"/>
-      <c r="S13" s="2">
-        <v>1</v>
-      </c>
-      <c r="T13" s="2">
+      <c r="S13" s="18"/>
+      <c r="T13" s="11">
         <v>1</v>
       </c>
       <c r="U13" s="12"/>
-      <c r="V13" s="2"/>
+      <c r="V13" s="4"/>
       <c r="W13" s="11">
         <v>1</v>
       </c>
-      <c r="X13" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2">
+      <c r="X13" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="12">
         <v>1</v>
       </c>
       <c r="AA13" s="2"/>
@@ -2354,9 +2345,7 @@
       <c r="AG13" s="2">
         <v>1</v>
       </c>
-      <c r="AH13" s="12">
-        <v>1</v>
-      </c>
+      <c r="AH13" s="12"/>
       <c r="AI13" s="2">
         <v>1</v>
       </c>
@@ -2364,188 +2353,105 @@
         <v>1</v>
       </c>
       <c r="AK13" s="2"/>
-      <c r="AL13" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM13" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN13" s="2"/>
+      <c r="AL13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="11"/>
       <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AR13" s="2"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
       <c r="AS13" s="17">
         <v>1</v>
       </c>
       <c r="AT13" s="17"/>
-      <c r="AU13" s="2">
+      <c r="AU13" s="11">
         <v>1</v>
       </c>
       <c r="AV13" s="18"/>
       <c r="AW13" s="18"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2"/>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="3">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="11">
-        <v>1</v>
-      </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="11">
-        <v>1</v>
-      </c>
-      <c r="U14" s="12"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="11">
-        <v>1</v>
-      </c>
-      <c r="X14" s="11">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH14" s="12"/>
-      <c r="AI14" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ14" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="11">
-        <v>1</v>
-      </c>
-      <c r="AM14" s="11">
-        <v>1</v>
-      </c>
-      <c r="AN14" s="11"/>
-      <c r="AO14" s="2"/>
-      <c r="AP14" s="4"/>
-      <c r="AQ14" s="4"/>
-      <c r="AR14" s="4"/>
+      <c r="I14" s="17">
+        <v>1</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="17">
+        <v>1</v>
+      </c>
+      <c r="O14" s="18"/>
+      <c r="P14" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="17">
+        <v>1</v>
+      </c>
+      <c r="T14" s="17">
+        <v>1</v>
+      </c>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="17">
+        <v>1</v>
+      </c>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="18"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="18"/>
+      <c r="AN14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="18"/>
+      <c r="AQ14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AR14" s="18"/>
       <c r="AS14" s="17">
         <v>1</v>
       </c>
-      <c r="AT14" s="17"/>
-      <c r="AU14" s="11">
-        <v>1</v>
-      </c>
-      <c r="AV14" s="18"/>
-      <c r="AW14" s="18"/>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="17">
-        <v>1</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="17">
-        <v>1</v>
-      </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="17">
-        <v>1</v>
-      </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="17">
-        <v>1</v>
-      </c>
-      <c r="T15" s="17">
-        <v>1</v>
-      </c>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="17">
-        <v>1</v>
-      </c>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="17"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="18"/>
-      <c r="AH15" s="18"/>
-      <c r="AI15" s="18"/>
-      <c r="AJ15" s="18"/>
-      <c r="AK15" s="18"/>
-      <c r="AL15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AM15" s="18"/>
-      <c r="AN15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AO15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AP15" s="18"/>
-      <c r="AQ15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AR15" s="18"/>
-      <c r="AS15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AT15" s="17">
-        <v>1</v>
-      </c>
-      <c r="AU15" s="17">
+      <c r="AT14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AU14" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2563,59 +2469,59 @@
       <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="14.75" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I11" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I12" s="22" t="s">
         <v>0</v>
       </c>
@@ -2623,103 +2529,103 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I13" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L13" s="32" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I14" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I15" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I16" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" t="s">
+    <row r="18" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I18" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" s="32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I18" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="L18" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I19" s="22" t="s">
         <v>4</v>
       </c>
       <c r="L19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I20" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I20" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="L20" t="s">
+    <row r="21" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I21" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="L21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I21" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I22" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I23" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="9:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="I24" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="9:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="I24" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I25" s="22" t="s">
         <v>9</v>
       </c>
@@ -2727,179 +2633,179 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I26" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I27" s="22" t="s">
         <v>41</v>
-      </c>
-      <c r="L26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I27" s="22" t="s">
-        <v>42</v>
       </c>
       <c r="L27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I28" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="9:12" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I29" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I30" s="22" t="s">
         <v>11</v>
       </c>
       <c r="L30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I31" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I31" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="L31" t="s">
+    <row r="32" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I32" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="L32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I32" s="22" t="s">
+    <row r="33" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I33" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L33" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I33" s="22" t="s">
+    <row r="34" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I34" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I35" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="L33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I34" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="L35" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I35" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="L35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I36" s="22" t="s">
         <v>14</v>
       </c>
       <c r="L36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I37" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="L37" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I37" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="L37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="9:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:12" ht="32" x14ac:dyDescent="0.2">
       <c r="I38" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I39" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I40" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="L40" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I40" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="L40" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I41" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I42" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L42" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="9:12" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I43" s="22" t="s">
         <v>17</v>
       </c>
       <c r="L43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I44" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="L44" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I44" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I45" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:12" x14ac:dyDescent="0.2">
       <c r="L46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L47" t="s">
+    <row r="48" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="L48" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L48" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>